<commit_message>
Layout and name updates
</commit_message>
<xml_diff>
--- a/The Web.xlsx
+++ b/The Web.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="164">
   <si>
     <t>from</t>
   </si>
@@ -343,55 +343,52 @@
     <t>Rosie Spencer</t>
   </si>
   <si>
+    <t>Rimicans</t>
+  </si>
+  <si>
+    <t>CITPA</t>
+  </si>
+  <si>
+    <t>Alice Wilson</t>
+  </si>
+  <si>
+    <t>Louis McMillan</t>
+  </si>
+  <si>
+    <t>Iris McMillan</t>
+  </si>
+  <si>
+    <t>Surface News</t>
+  </si>
+  <si>
+    <t>Amelie Dryer</t>
+  </si>
+  <si>
+    <t>Saskia Chaplin</t>
+  </si>
+  <si>
+    <t>Fredie Fearn</t>
+  </si>
+  <si>
+    <t>Finlay RD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finlay RD </t>
+  </si>
+  <si>
+    <t>Charity Tweaks</t>
+  </si>
+  <si>
     <t>Gay Barber</t>
   </si>
   <si>
-    <t>Rimicans</t>
-  </si>
-  <si>
-    <t>CITPA</t>
-  </si>
-  <si>
-    <t>Peter Molloy</t>
-  </si>
-  <si>
-    <t>Alice Wilson</t>
-  </si>
-  <si>
-    <t>Louis McMillan</t>
-  </si>
-  <si>
-    <t>Iris McMillan</t>
-  </si>
-  <si>
-    <t>Surface News</t>
-  </si>
-  <si>
-    <t>Amelie Dryer</t>
-  </si>
-  <si>
-    <t>Saskia Chaplin</t>
-  </si>
-  <si>
-    <t>Fredie Fearn</t>
-  </si>
-  <si>
-    <t>Finlay RD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finlay RD </t>
-  </si>
-  <si>
-    <t>Charity Tweaks</t>
-  </si>
-  <si>
     <t>Stan Heap</t>
   </si>
   <si>
     <t>Alisson Bell</t>
   </si>
   <si>
-    <t>Hog Barrie</t>
+    <t>Waltuh Hog Barrie</t>
   </si>
   <si>
     <t>Emma Crawford</t>
@@ -3355,7 +3352,7 @@
         <v>109</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="C146" s="7" t="s">
         <v>12</v>
@@ -3372,7 +3369,7 @@
         <v>109</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C147" s="7" t="s">
         <v>12</v>
@@ -3406,7 +3403,7 @@
         <v>32</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C149" s="6" t="s">
         <v>10</v>
@@ -3420,10 +3417,10 @@
     </row>
     <row r="150" ht="15.75" customHeight="1">
       <c r="A150" s="8" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="B150" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C150" s="7" t="s">
         <v>12</v>
@@ -3437,10 +3434,10 @@
     </row>
     <row r="151" ht="15.75" customHeight="1">
       <c r="A151" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B151" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C151" s="7" t="s">
         <v>12</v>
@@ -3457,7 +3454,7 @@
         <v>99</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C152" s="6" t="s">
         <v>10</v>
@@ -3505,10 +3502,10 @@
     </row>
     <row r="155" ht="15.75" customHeight="1">
       <c r="A155" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C155" s="6" t="s">
         <v>10</v>
@@ -3522,10 +3519,10 @@
     </row>
     <row r="156" ht="15.75" customHeight="1">
       <c r="A156" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C156" s="6" t="s">
         <v>10</v>
@@ -3539,10 +3536,10 @@
     </row>
     <row r="157" ht="15.75" customHeight="1">
       <c r="A157" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B157" s="8" t="s">
         <v>119</v>
-      </c>
-      <c r="B157" s="8" t="s">
-        <v>121</v>
       </c>
       <c r="C157" s="7" t="s">
         <v>12</v>
@@ -3556,7 +3553,7 @@
     </row>
     <row r="158" ht="15.75" customHeight="1">
       <c r="A158" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B158" s="8" t="s">
         <v>103</v>
@@ -3573,10 +3570,10 @@
     </row>
     <row r="159" ht="15.75" customHeight="1">
       <c r="A159" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C159" s="7" t="s">
         <v>12</v>
@@ -3590,7 +3587,7 @@
     </row>
     <row r="160" ht="15.75" customHeight="1">
       <c r="A160" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B160" s="8" t="s">
         <v>6</v>
@@ -3607,10 +3604,10 @@
     </row>
     <row r="161" ht="15.75" customHeight="1">
       <c r="A161" s="8" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C161" s="7" t="s">
         <v>12</v>
@@ -3624,10 +3621,10 @@
     </row>
     <row r="162" ht="15.75" customHeight="1">
       <c r="A162" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C162" s="7" t="s">
         <v>12</v>
@@ -3641,10 +3638,10 @@
     </row>
     <row r="163" ht="15.75" customHeight="1">
       <c r="A163" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B163" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="B163" s="8" t="s">
-        <v>127</v>
       </c>
       <c r="C163" s="6" t="s">
         <v>10</v>
@@ -3678,7 +3675,7 @@
         <v>39</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C165" s="7" t="s">
         <v>12</v>
@@ -3712,7 +3709,7 @@
         <v>39</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C167" s="7" t="s">
         <v>12</v>
@@ -3726,10 +3723,10 @@
     </row>
     <row r="168" ht="15.75" customHeight="1">
       <c r="A168" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B168" s="8" t="s">
         <v>129</v>
-      </c>
-      <c r="B168" s="8" t="s">
-        <v>130</v>
       </c>
       <c r="C168" s="6" t="s">
         <v>10</v>
@@ -3743,10 +3740,10 @@
     </row>
     <row r="169" ht="15.75" customHeight="1">
       <c r="A169" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C169" s="6" t="s">
         <v>10</v>
@@ -3760,7 +3757,7 @@
     </row>
     <row r="170" ht="15.75" customHeight="1">
       <c r="A170" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B170" s="8" t="s">
         <v>93</v>
@@ -3777,10 +3774,10 @@
     </row>
     <row r="171" ht="15.75" customHeight="1">
       <c r="A171" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B171" s="8" t="s">
         <v>131</v>
-      </c>
-      <c r="B171" s="8" t="s">
-        <v>132</v>
       </c>
       <c r="C171" s="7" t="s">
         <v>12</v>
@@ -3797,7 +3794,7 @@
         <v>50</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C172" s="6" t="s">
         <v>10</v>
@@ -3814,7 +3811,7 @@
         <v>9</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C173" s="7" t="s">
         <v>12</v>
@@ -3831,7 +3828,7 @@
         <v>24</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C174" s="7" t="s">
         <v>12</v>
@@ -3848,7 +3845,7 @@
         <v>24</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C175" s="7" t="s">
         <v>12</v>
@@ -3865,7 +3862,7 @@
         <v>106</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C176" s="4" t="s">
         <v>7</v>
@@ -3882,7 +3879,7 @@
         <v>87</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C177" s="7" t="s">
         <v>12</v>
@@ -3896,10 +3893,10 @@
     </row>
     <row r="178" ht="15.75" customHeight="1">
       <c r="A178" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C178" s="6" t="s">
         <v>10</v>
@@ -3916,7 +3913,7 @@
         <v>74</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C179" s="7" t="s">
         <v>12</v>
@@ -3947,7 +3944,7 @@
     </row>
     <row r="181" ht="15.75" customHeight="1">
       <c r="A181" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B181" s="8" t="s">
         <v>75</v>
@@ -3964,7 +3961,7 @@
     </row>
     <row r="182" ht="15.75" customHeight="1">
       <c r="A182" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B182" s="8" t="s">
         <v>15</v>
@@ -3981,7 +3978,7 @@
     </row>
     <row r="183" ht="15.75" customHeight="1">
       <c r="A183" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B183" s="8" t="s">
         <v>106</v>
@@ -4018,7 +4015,7 @@
         <v>72</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C185" s="6" t="s">
         <v>10</v>
@@ -4083,7 +4080,7 @@
     </row>
     <row r="189" ht="15.75" customHeight="1">
       <c r="A189" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B189" s="8" t="s">
         <v>5</v>
@@ -4100,10 +4097,10 @@
     </row>
     <row r="190" ht="15.75" customHeight="1">
       <c r="A190" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B190" s="8" t="s">
         <v>142</v>
-      </c>
-      <c r="B190" s="8" t="s">
-        <v>143</v>
       </c>
       <c r="C190" s="4" t="s">
         <v>7</v>
@@ -4120,7 +4117,7 @@
         <v>93</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C191" s="7" t="s">
         <v>12</v>
@@ -4134,7 +4131,7 @@
     </row>
     <row r="192" ht="15.75" customHeight="1">
       <c r="A192" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B192" s="8" t="s">
         <v>63</v>
@@ -4151,7 +4148,7 @@
     </row>
     <row r="193" ht="15.75" customHeight="1">
       <c r="A193" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B193" s="8" t="s">
         <v>18</v>
@@ -4168,10 +4165,10 @@
     </row>
     <row r="194" ht="15.75" customHeight="1">
       <c r="A194" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B194" s="8" t="s">
         <v>145</v>
-      </c>
-      <c r="B194" s="8" t="s">
-        <v>146</v>
       </c>
       <c r="C194" s="6" t="s">
         <v>10</v>
@@ -4188,7 +4185,7 @@
         <v>44</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C195" s="6" t="s">
         <v>10</v>
@@ -4222,7 +4219,7 @@
         <v>35</v>
       </c>
       <c r="B197" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C197" s="6" t="s">
         <v>10</v>
@@ -4239,7 +4236,7 @@
         <v>57</v>
       </c>
       <c r="B198" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C198" s="7" t="s">
         <v>12</v>
@@ -4273,7 +4270,7 @@
         <v>34</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C200" s="6" t="s">
         <v>10</v>
@@ -4287,10 +4284,10 @@
     </row>
     <row r="201" ht="15.75" customHeight="1">
       <c r="A201" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C201" s="6" t="s">
         <v>10</v>
@@ -4321,10 +4318,10 @@
     </row>
     <row r="203" ht="15.75" customHeight="1">
       <c r="A203" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B203" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="B203" s="8" t="s">
-        <v>151</v>
       </c>
       <c r="C203" s="6" t="s">
         <v>10</v>
@@ -4338,10 +4335,10 @@
     </row>
     <row r="204" ht="15.75" customHeight="1">
       <c r="A204" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B204" s="8" t="s">
         <v>152</v>
-      </c>
-      <c r="B204" s="8" t="s">
-        <v>153</v>
       </c>
       <c r="C204" s="7" t="s">
         <v>12</v>
@@ -4389,7 +4386,7 @@
     </row>
     <row r="207" ht="15.75" customHeight="1">
       <c r="A207" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B207" s="8" t="s">
         <v>84</v>
@@ -4406,7 +4403,7 @@
     </row>
     <row r="208" ht="15.75" customHeight="1">
       <c r="A208" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B208" s="8" t="s">
         <v>84</v>
@@ -4440,7 +4437,7 @@
     </row>
     <row r="210" ht="15.75" customHeight="1">
       <c r="A210" s="8" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="B210" s="8" t="s">
         <v>84</v>
@@ -4460,7 +4457,7 @@
         <v>92</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C211" s="6" t="s">
         <v>10</v>
@@ -4483,7 +4480,7 @@
         <v>12</v>
       </c>
       <c r="D212" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E212" s="5" t="s">
         <v>8</v>
@@ -4491,10 +4488,10 @@
     </row>
     <row r="213" ht="15.75" customHeight="1">
       <c r="A213" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B213" s="8" t="s">
         <v>157</v>
-      </c>
-      <c r="B213" s="8" t="s">
-        <v>158</v>
       </c>
       <c r="C213" s="7" t="s">
         <v>12</v>
@@ -4508,13 +4505,13 @@
     </row>
     <row r="214" ht="15.75" customHeight="1">
       <c r="A214" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B214" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C214" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D214" s="5" t="s">
         <v>8</v>
@@ -4525,7 +4522,7 @@
     </row>
     <row r="215" ht="15.75" customHeight="1">
       <c r="A215" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B215" s="8" t="s">
         <v>88</v>
@@ -4542,13 +4539,13 @@
     </row>
     <row r="216" ht="15.75" customHeight="1">
       <c r="A216" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B216" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C216" s="13" t="s">
         <v>161</v>
-      </c>
-      <c r="C216" s="13" t="s">
-        <v>162</v>
       </c>
       <c r="D216" s="9" t="s">
         <v>20</v>
@@ -4559,10 +4556,10 @@
     </row>
     <row r="217" ht="15.75" customHeight="1">
       <c r="A217" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C217" s="7" t="s">
         <v>12</v>
@@ -4576,10 +4573,10 @@
     </row>
     <row r="218" ht="15.75" customHeight="1">
       <c r="A218" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B218" s="8" t="s">
         <v>163</v>
-      </c>
-      <c r="B218" s="8" t="s">
-        <v>164</v>
       </c>
       <c r="C218" s="4" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Formatting and layout changes
</commit_message>
<xml_diff>
--- a/The Web.xlsx
+++ b/The Web.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="162">
   <si>
     <t>from</t>
   </si>
@@ -160,7 +160,7 @@
     <t>Holly Stodgell</t>
   </si>
   <si>
-    <t>Alison Bell</t>
+    <t>Alisson Bell</t>
   </si>
   <si>
     <t>Emma Halliwell</t>
@@ -190,7 +190,7 @@
     <t>Eddie Narbett</t>
   </si>
   <si>
-    <t>Sasha Cheplin</t>
+    <t>Sasha Chepelin</t>
   </si>
   <si>
     <t>Freddie Carcas</t>
@@ -352,9 +352,6 @@
     <t>Alice Wilson</t>
   </si>
   <si>
-    <t>Louis McMillan</t>
-  </si>
-  <si>
     <t>Iris McMillan</t>
   </si>
   <si>
@@ -379,15 +376,9 @@
     <t>Charity Tweaks</t>
   </si>
   <si>
-    <t>Gay Barber</t>
-  </si>
-  <si>
     <t>Stan Heap</t>
   </si>
   <si>
-    <t>Alisson Bell</t>
-  </si>
-  <si>
     <t>Waltuh Hog Barrie</t>
   </si>
   <si>
@@ -445,9 +436,6 @@
     <t>Finlay Todd</t>
   </si>
   <si>
-    <t>Sasha Chepelin</t>
-  </si>
-  <si>
     <t>Jura McMillan</t>
   </si>
   <si>
@@ -503,6 +491,12 @@
   </si>
   <si>
     <t>Heidi Robertshaw</t>
+  </si>
+  <si>
+    <t>Maja Thomson</t>
+  </si>
+  <si>
+    <t>Euan Patton</t>
   </si>
 </sst>
 </file>
@@ -3434,7 +3428,7 @@
     </row>
     <row r="151" ht="15.75" customHeight="1">
       <c r="A151" s="8" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
       <c r="B151" s="8" t="s">
         <v>112</v>
@@ -3454,7 +3448,7 @@
         <v>99</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C152" s="6" t="s">
         <v>10</v>
@@ -3502,10 +3496,10 @@
     </row>
     <row r="155" ht="15.75" customHeight="1">
       <c r="A155" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B155" s="8" t="s">
         <v>115</v>
-      </c>
-      <c r="B155" s="8" t="s">
-        <v>116</v>
       </c>
       <c r="C155" s="6" t="s">
         <v>10</v>
@@ -3519,10 +3513,10 @@
     </row>
     <row r="156" ht="15.75" customHeight="1">
       <c r="A156" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B156" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="B156" s="8" t="s">
-        <v>118</v>
       </c>
       <c r="C156" s="6" t="s">
         <v>10</v>
@@ -3536,10 +3530,10 @@
     </row>
     <row r="157" ht="15.75" customHeight="1">
       <c r="A157" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C157" s="7" t="s">
         <v>12</v>
@@ -3553,7 +3547,7 @@
     </row>
     <row r="158" ht="15.75" customHeight="1">
       <c r="A158" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B158" s="8" t="s">
         <v>103</v>
@@ -3570,10 +3564,10 @@
     </row>
     <row r="159" ht="15.75" customHeight="1">
       <c r="A159" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B159" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="B159" s="8" t="s">
-        <v>121</v>
       </c>
       <c r="C159" s="7" t="s">
         <v>12</v>
@@ -3587,7 +3581,7 @@
     </row>
     <row r="160" ht="15.75" customHeight="1">
       <c r="A160" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B160" s="8" t="s">
         <v>6</v>
@@ -3604,10 +3598,10 @@
     </row>
     <row r="161" ht="15.75" customHeight="1">
       <c r="A161" s="8" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C161" s="7" t="s">
         <v>12</v>
@@ -3621,10 +3615,10 @@
     </row>
     <row r="162" ht="15.75" customHeight="1">
       <c r="A162" s="8" t="s">
-        <v>124</v>
+        <v>49</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C162" s="7" t="s">
         <v>12</v>
@@ -3638,10 +3632,10 @@
     </row>
     <row r="163" ht="15.75" customHeight="1">
       <c r="A163" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C163" s="6" t="s">
         <v>10</v>
@@ -3675,7 +3669,7 @@
         <v>39</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C165" s="7" t="s">
         <v>12</v>
@@ -3709,7 +3703,7 @@
         <v>39</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C167" s="7" t="s">
         <v>12</v>
@@ -3723,10 +3717,10 @@
     </row>
     <row r="168" ht="15.75" customHeight="1">
       <c r="A168" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C168" s="6" t="s">
         <v>10</v>
@@ -3740,10 +3734,10 @@
     </row>
     <row r="169" ht="15.75" customHeight="1">
       <c r="A169" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C169" s="6" t="s">
         <v>10</v>
@@ -3757,7 +3751,7 @@
     </row>
     <row r="170" ht="15.75" customHeight="1">
       <c r="A170" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B170" s="8" t="s">
         <v>93</v>
@@ -3774,10 +3768,10 @@
     </row>
     <row r="171" ht="15.75" customHeight="1">
       <c r="A171" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C171" s="7" t="s">
         <v>12</v>
@@ -3794,7 +3788,7 @@
         <v>50</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C172" s="6" t="s">
         <v>10</v>
@@ -3811,7 +3805,7 @@
         <v>9</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C173" s="7" t="s">
         <v>12</v>
@@ -3828,7 +3822,7 @@
         <v>24</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C174" s="7" t="s">
         <v>12</v>
@@ -3845,7 +3839,7 @@
         <v>24</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C175" s="7" t="s">
         <v>12</v>
@@ -3862,7 +3856,7 @@
         <v>106</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C176" s="4" t="s">
         <v>7</v>
@@ -3879,7 +3873,7 @@
         <v>87</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C177" s="7" t="s">
         <v>12</v>
@@ -3893,10 +3887,10 @@
     </row>
     <row r="178" ht="15.75" customHeight="1">
       <c r="A178" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C178" s="6" t="s">
         <v>10</v>
@@ -3913,7 +3907,7 @@
         <v>74</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C179" s="7" t="s">
         <v>12</v>
@@ -3944,7 +3938,7 @@
     </row>
     <row r="181" ht="15.75" customHeight="1">
       <c r="A181" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B181" s="8" t="s">
         <v>75</v>
@@ -3961,7 +3955,7 @@
     </row>
     <row r="182" ht="15.75" customHeight="1">
       <c r="A182" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B182" s="8" t="s">
         <v>15</v>
@@ -3978,7 +3972,7 @@
     </row>
     <row r="183" ht="15.75" customHeight="1">
       <c r="A183" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B183" s="8" t="s">
         <v>106</v>
@@ -4015,7 +4009,7 @@
         <v>72</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C185" s="6" t="s">
         <v>10</v>
@@ -4080,7 +4074,7 @@
     </row>
     <row r="189" ht="15.75" customHeight="1">
       <c r="A189" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B189" s="8" t="s">
         <v>5</v>
@@ -4097,10 +4091,10 @@
     </row>
     <row r="190" ht="15.75" customHeight="1">
       <c r="A190" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C190" s="4" t="s">
         <v>7</v>
@@ -4117,7 +4111,7 @@
         <v>93</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C191" s="7" t="s">
         <v>12</v>
@@ -4131,7 +4125,7 @@
     </row>
     <row r="192" ht="15.75" customHeight="1">
       <c r="A192" s="8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B192" s="8" t="s">
         <v>63</v>
@@ -4148,7 +4142,7 @@
     </row>
     <row r="193" ht="15.75" customHeight="1">
       <c r="A193" s="8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B193" s="8" t="s">
         <v>18</v>
@@ -4165,10 +4159,10 @@
     </row>
     <row r="194" ht="15.75" customHeight="1">
       <c r="A194" s="8" t="s">
-        <v>144</v>
+        <v>59</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C194" s="6" t="s">
         <v>10</v>
@@ -4185,7 +4179,7 @@
         <v>44</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C195" s="6" t="s">
         <v>10</v>
@@ -4219,7 +4213,7 @@
         <v>35</v>
       </c>
       <c r="B197" s="8" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C197" s="6" t="s">
         <v>10</v>
@@ -4236,7 +4230,7 @@
         <v>57</v>
       </c>
       <c r="B198" s="8" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C198" s="7" t="s">
         <v>12</v>
@@ -4270,7 +4264,7 @@
         <v>34</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C200" s="6" t="s">
         <v>10</v>
@@ -4284,10 +4278,10 @@
     </row>
     <row r="201" ht="15.75" customHeight="1">
       <c r="A201" s="8" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C201" s="6" t="s">
         <v>10</v>
@@ -4318,10 +4312,10 @@
     </row>
     <row r="203" ht="15.75" customHeight="1">
       <c r="A203" s="8" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B203" s="8" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C203" s="6" t="s">
         <v>10</v>
@@ -4335,10 +4329,10 @@
     </row>
     <row r="204" ht="15.75" customHeight="1">
       <c r="A204" s="8" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C204" s="7" t="s">
         <v>12</v>
@@ -4386,7 +4380,7 @@
     </row>
     <row r="207" ht="15.75" customHeight="1">
       <c r="A207" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B207" s="8" t="s">
         <v>84</v>
@@ -4403,7 +4397,7 @@
     </row>
     <row r="208" ht="15.75" customHeight="1">
       <c r="A208" s="8" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B208" s="8" t="s">
         <v>84</v>
@@ -4457,7 +4451,7 @@
         <v>92</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C211" s="6" t="s">
         <v>10</v>
@@ -4480,7 +4474,7 @@
         <v>12</v>
       </c>
       <c r="D212" s="7" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E212" s="5" t="s">
         <v>8</v>
@@ -4488,10 +4482,10 @@
     </row>
     <row r="213" ht="15.75" customHeight="1">
       <c r="A213" s="8" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B213" s="8" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C213" s="7" t="s">
         <v>12</v>
@@ -4505,13 +4499,13 @@
     </row>
     <row r="214" ht="15.75" customHeight="1">
       <c r="A214" s="8" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B214" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C214" s="11" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D214" s="5" t="s">
         <v>8</v>
@@ -4522,7 +4516,7 @@
     </row>
     <row r="215" ht="15.75" customHeight="1">
       <c r="A215" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B215" s="8" t="s">
         <v>88</v>
@@ -4539,13 +4533,13 @@
     </row>
     <row r="216" ht="15.75" customHeight="1">
       <c r="A216" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B216" s="8" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C216" s="13" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D216" s="9" t="s">
         <v>20</v>
@@ -4556,10 +4550,10 @@
     </row>
     <row r="217" ht="15.75" customHeight="1">
       <c r="A217" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C217" s="7" t="s">
         <v>12</v>
@@ -4573,10 +4567,10 @@
     </row>
     <row r="218" ht="15.75" customHeight="1">
       <c r="A218" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B218" s="8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C218" s="4" t="s">
         <v>7</v>
@@ -4588,8 +4582,40 @@
         <v>20</v>
       </c>
     </row>
-    <row r="219" ht="15.75" customHeight="1"/>
-    <row r="220" ht="15.75" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1">
+      <c r="A219" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B219" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C219" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D219" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E219" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="220" ht="15.75" customHeight="1">
+      <c r="A220" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B220" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C220" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D220" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E220" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="221" ht="15.75" customHeight="1"/>
     <row r="222" ht="15.75" customHeight="1"/>
     <row r="223" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
updates - people mad at web :(.
</commit_message>
<xml_diff>
--- a/The Web.xlsx
+++ b/The Web.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="237">
   <si>
     <t>from</t>
   </si>
@@ -571,18 +571,24 @@
     <t>Mhairi Ballantyne</t>
   </si>
   <si>
+    <t>Bezza Pezza</t>
+  </si>
+  <si>
+    <t>Bish</t>
+  </si>
+  <si>
+    <t>Karoline</t>
+  </si>
+  <si>
     <t>Laurence Ward</t>
   </si>
   <si>
-    <t>Bish</t>
-  </si>
-  <si>
-    <t>Karoline</t>
-  </si>
-  <si>
     <t>Daisy Rennie</t>
   </si>
   <si>
+    <t xml:space="preserve">Isaac Hunter </t>
+  </si>
+  <si>
     <t>Female</t>
   </si>
   <si>
@@ -668,12 +674,6 @@
   </si>
   <si>
     <t xml:space="preserve">New SEO description </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isaac Hunter </t>
-  </si>
-  <si>
-    <t>Bezza Pezza</t>
   </si>
   <si>
     <t xml:space="preserve">Loosy </t>
@@ -843,7 +843,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -908,20 +908,8 @@
     <xf borderId="0" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2618,8 +2606,8 @@
       <c r="B86" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C86" s="6" t="s">
-        <v>10</v>
+      <c r="C86" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>8</v>
@@ -5413,13 +5401,13 @@
         <v>185</v>
       </c>
       <c r="B250" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="C250" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D250" s="5" t="s">
-        <v>8</v>
+        <v>183</v>
+      </c>
+      <c r="C250" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D250" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="E250" s="9" t="s">
         <v>20</v>
@@ -5461,10 +5449,10 @@
     </row>
     <row r="253" ht="15.75" customHeight="1">
       <c r="A253" s="8" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B253" s="8" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C253" s="6" t="s">
         <v>10</v>
@@ -5477,24 +5465,60 @@
       </c>
     </row>
     <row r="254" ht="15.75" customHeight="1">
-      <c r="C254" s="4"/>
-      <c r="D254" s="10"/>
-      <c r="E254" s="10"/>
+      <c r="A254" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B254" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C254" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D254" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E254" s="10" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="255" ht="15.75" customHeight="1">
-      <c r="C255" s="4"/>
-      <c r="D255" s="5"/>
-      <c r="E255" s="5"/>
+      <c r="A255" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B255" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C255" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D255" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E255" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="256" ht="15.75" customHeight="1">
-      <c r="C256" s="4"/>
-      <c r="D256" s="10"/>
-      <c r="E256" s="5"/>
+      <c r="A256" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B256" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C256" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D256" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E256" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="257" ht="15.75" customHeight="1">
-      <c r="C257" s="7"/>
-      <c r="D257" s="10"/>
-      <c r="E257" s="9"/>
+      <c r="C257" s="22"/>
+      <c r="D257" s="22"/>
+      <c r="E257" s="22"/>
     </row>
     <row r="258" ht="15.75" customHeight="1"/>
     <row r="259" ht="15.75" customHeight="1"/>
@@ -6279,21 +6303,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="8" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>43</v>
@@ -6307,7 +6331,7 @@
         <v>13</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4">
@@ -6326,18 +6350,18 @@
         <v>15</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="8" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>54</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7">
@@ -6348,15 +6372,15 @@
         <v>79</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="8" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9">
@@ -6367,7 +6391,7 @@
         <v>31</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10">
@@ -6410,7 +6434,7 @@
         <v>55</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15">
@@ -6450,7 +6474,7 @@
         <v>88</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="20">
@@ -6474,7 +6498,7 @@
         <v>32</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="23">
@@ -6482,7 +6506,7 @@
         <v>116</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24">
@@ -6495,7 +6519,7 @@
     </row>
     <row r="25">
       <c r="A25" s="8" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>59</v>
@@ -6554,7 +6578,7 @@
         <v>108</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33">
@@ -6575,10 +6599,10 @@
     </row>
     <row r="35">
       <c r="A35" s="8" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36">
@@ -6607,7 +6631,7 @@
     </row>
     <row r="39">
       <c r="A39" s="8" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>99</v>
@@ -6615,7 +6639,7 @@
     </row>
     <row r="40">
       <c r="A40" s="8" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>33</v>
@@ -6690,7 +6714,7 @@
         <v>36</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="50">
@@ -6839,7 +6863,7 @@
     </row>
     <row r="68">
       <c r="D68" s="8" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="69">
@@ -6854,12 +6878,12 @@
     </row>
     <row r="71">
       <c r="D71" s="8" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="72">
       <c r="D72" s="8" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="73">
@@ -6902,85 +6926,17 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="8" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="8" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="16" t="s">
-        <v>218</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="16" t="s">
         <v>219</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>